<commit_message>
Atualização automática de SAO_LOURENCO_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/SAO_LOURENCO_DO_SUL.xlsx
+++ b/SAO_LOURENCO_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A25985EA-2F47-43CB-BB93-E9356BEF16F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1C1496A9-347B-4302-88A5-9DC356AB6917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1374,7 +1374,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{B4B8D7B7-F1F9-4BD0-BD05-E57E3214AEBB}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{C11AE8B9-A535-4246-A92C-2C708A5CC03C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1404,10 +1404,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F6958F5-9056-45C8-A42C-51C1BE1738F5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84786F73-8D86-47C1-844E-E3D7E16F2EDA}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1445,7 +1445,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AE39E0A-6787-4137-8F60-206249DD5482}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DCCB457-FEC4-4FAE-9002-E01A42AC3ADC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1508,7 +1508,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1F8B830-23A4-4E02-BD07-E500BFC92C08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EC4A6BE-1E85-45E4-8B1D-6A09FD10904C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1527,7 +1527,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13D4F8F6-7365-4A13-3AC6-0ABD407CA7F2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03F2159B-4268-D1C9-37B7-8091456DDCB4}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1576,7 +1576,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9701C82-A9AF-01C4-C584-C15BCC0A5EE2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C5C718E-F555-0C2B-EA19-3E6281F19E1A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1595,7 +1595,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0615FCDC-DE74-FA90-1AD0-2D1F971F86B7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD0420DC-F3A1-D481-D7DB-26509FEA00D1}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1626,7 +1626,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5E723E2-B661-907F-C74C-D7CD515048D7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C56EC542-43E4-7707-C3D6-1E6832572CB8}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1657,7 +1657,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A07D53C-6576-B86D-75E4-0A77DA45E3AC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D0CA40E-0CD9-8419-39ED-CB3122DEC831}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1700,7 +1700,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E7B646B-90CF-404B-AC12-E6C4C82D5EA1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A55F20D-461C-40F5-8D16-3F043F56BB6D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1738,7 +1738,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{431B6559-7D7D-4E5D-8C5C-9C09C8C16417}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68AFE3D4-ADCC-4C78-980F-2205158BA013}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1781,7 +1781,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAEE1598-D06E-4C57-8020-92C8C9D05432}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3AF9FA8B-0290-4FE4-AE0F-88C1E5CCA704}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2094,7 +2094,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16BF4C35-A210-4A87-B6DC-19E48C03F7C5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{358A1775-8583-4922-899B-40256C252804}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>